<commit_message>
added extra new results from spider 2
</commit_message>
<xml_diff>
--- a/ZorgkaartScrapy/data/zorgkaart_organisaties.xlsx
+++ b/ZorgkaartScrapy/data/zorgkaart_organisaties.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:C121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2150,6 +2150,346 @@
         </is>
       </c>
     </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Staas &amp; Bergmans, locatie Groote Wielen</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-staas-bergmans-locatie-groote-wielen-rosmalen-10025334</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Tandarts Abas</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandarts-abas-bussum-3054204</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>De Kliniek voor Tandheelkunde</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-de-kliniek-voor-tandheelkunde-utrecht-182964</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Dijkstra &amp; De Wet Tandheelkunde</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dijkstra-de-wet-tandheelkunde-amsterdam-10020311</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Amstel Dental - Tandarts Bussum</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-amstel-dental-tandarts-bussum-bussum-10021599</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Dental Clinics Oldenzaal</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-oldenzaal-oldenzaal-3048472</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Venema tandartsen</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-venema-tandartsen-helmond-185417</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>KT3 tandartspraktijk</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-kt3-tandartspraktijk-zaandam-180596</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Tandartspraktijk Romero</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartspraktijk-romero-honselersdijk-10027597</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>De Tandarts, kliniek voor tandheelkunde en implantologie</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-de-tandarts-kliniek-voor-tandheelkunde-en-implantologie-raamsdonksveer-184568</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Operatandarts de By &amp; de By</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-operatandarts-de-by-de-by-amsterdam-209685</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Mondzorg Oosterhout</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-mondzorg-oosterhout-oosterhout-10026683</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Tandartsenpraktijk Paul en de Witte</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartsenpraktijk-paul-en-de-witte-vlissingen-184137</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Tandheelkunde Beverdam</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandheelkunde-beverdam-wierden-3036333</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Dental Clinics Zaltbommel</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-zaltbommel-zaltbommel-208738</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Tandartsenpraktijk Grou</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartsenpraktijk-grou-grou-188160</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Dental Clinics Gouda Greenline</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-gouda-greenline-gouda-182093</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>PC2-tandartsen</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-pc2-tandartsen-eindhoven-3032943</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Dental Clinics Beuningen</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-beuningen-beuningen-3046007</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Dental Clinics Colmschate</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-colmschate-colmschate-187204</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
refactor spider with async start method, improved pagination logic, and error handling for max\_page
</commit_message>
<xml_diff>
--- a/ZorgkaartScrapy/data/zorgkaart_organisaties.xlsx
+++ b/ZorgkaartScrapy/data/zorgkaart_organisaties.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C121"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1470,1026 +1470,6 @@
         </is>
       </c>
     </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>Paro Praktijk Utrecht</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-paro-praktijk-utrecht-utrecht-181319</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>Mondzorg Scheveningen</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-mondzorg-scheveningen-den-haag-10013707</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>Tandarts Smile</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandarts-smile-nijmegen-3047171</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>JTVmondzorgvoorkids.nl, locatie Rotterdam, Rusthoflaan</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-jtvmondzorgvoorkids-nl-locatie-rotterdam-rusthoflaan-rotterdam-3048884</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>Tandheelkundig Centrum Molenvliet</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandheelkundig-centrum-molenvliet-alphen-aan-den-rijn-3025467</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>Dental Clinics Doetinchem - Lohmanlaan</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-doetinchem-lohmanlaan-doetinchem-186893</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>Dental Clinics Venlo</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-venlo-venlo-238125</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>Dental Clinics Rolde</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-rolde-rolde-3033445</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>Dental Clinics Zoetermeer Nabij</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-zoetermeer-nabij-zoetermeer-3033668</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>Dental Clinics Ridderkerk</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-ridderkerk-ridderkerk-182203</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>Dental Clinics Weesp</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-weesp-weesp-179876</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>Dental Clinics Rijswijk</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-rijswijk-rijswijk-3046612</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>Dental Clinics Oudenbosch</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-oudenbosch-oudenbosch-184534</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>Dental Clinics Hoogezand</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-hoogezand-hoogezand-3029572</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>Mondzorgcentrum de Parel</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-mondzorgcentrum-de-parel-oisterwijk-184680</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>Dental Clinics Barendrecht</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-barendrecht-barendrecht-239259</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>Dental Clinics Den Haag - Laan van Meerdervoort</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-den-haag-laan-van-meerdervoort-den-haag-3040988</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>Tandartspraktijk De Biezenkamp</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartspraktijk-de-biezenkamp-leusden-3047069</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>Dental Clinics Gieten</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-gieten-gieten-187591</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>Dental Clinics Zoetermeer Seghwaert</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-zoetermeer-seghwaert-zoetermeer-3007875</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>Dental Clinics Dordrecht Kuipershaven</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-dordrecht-kuipershaven-dordrecht-182817</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>Tandzuiver</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandzuiver-heemstede-3033317</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>Bolwerk Tandartsen</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-bolwerk-tandartsen-maastricht-224584</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>Botman tandartsen, locatie Blerick</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-botman-tandartsen-locatie-blerick-venlo-185540</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>Tandheelkundig Centrum 't Gooi</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandheelkundig-centrum-t-gooi-bussum-3033487</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>The Dentist Amsterdam</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-the-dentist-amsterdam-amsterdam-3054487</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>Tandartsenpraktijk Dental Luxe</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartsenpraktijk-dental-luxe-zoetermeer-3050548</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>Poorter Tandartsen</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-poorter-tandartsen-zoetermeer-3057904</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>Tandartspraktijk van de Sande</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartspraktijk-van-de-sande-teteringen-184477</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>Tandartspraktijk Gezondheidscentrum Jol</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartspraktijk-gezondheidscentrum-jol-lelystad-187887</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>Dental Clinics Oss</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-oss-oss-3041598</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>Espenbos Kliniek</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-espenbos-kliniek-cadier-en-keer-10013572</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>Dental Clinics Vught</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-vught-vught-184886</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>MakDo Mondzorgpraktijk, locatie Hoek</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-makdo-mondzorgpraktijk-locatie-hoek-hoek-184186</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>Dental Clinics Enschede Stokhorst &amp; Breuch</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-enschede-stokhorst-breuch-enschede-10020988</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>Dental Clinics Wassenaar</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-wassenaar-wassenaar-10022824</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>Tandartsengroepspraktijk Heemskerk</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartsengroepspraktijk-heemskerk-heemskerk-180618</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>Dental Clinics Leusden</t>
-        </is>
-      </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-leusden-leusden-10018142</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>Tandartsenpraktijk Belcrum</t>
-        </is>
-      </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartsenpraktijk-belcrum-breda-10021708</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>Tandartsenpraktijk TAND150</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartsenpraktijk-tand150-amsterdam-3043057</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>Staas &amp; Bergmans, locatie Groote Wielen</t>
-        </is>
-      </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-staas-bergmans-locatie-groote-wielen-rosmalen-10025334</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>Tandarts Abas</t>
-        </is>
-      </c>
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandarts-abas-bussum-3054204</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>De Kliniek voor Tandheelkunde</t>
-        </is>
-      </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-de-kliniek-voor-tandheelkunde-utrecht-182964</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>Dijkstra &amp; De Wet Tandheelkunde</t>
-        </is>
-      </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dijkstra-de-wet-tandheelkunde-amsterdam-10020311</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>Amstel Dental - Tandarts Bussum</t>
-        </is>
-      </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-amstel-dental-tandarts-bussum-bussum-10021599</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>Dental Clinics Oldenzaal</t>
-        </is>
-      </c>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-oldenzaal-oldenzaal-3048472</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>Venema tandartsen</t>
-        </is>
-      </c>
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-venema-tandartsen-helmond-185417</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>KT3 tandartspraktijk</t>
-        </is>
-      </c>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-kt3-tandartspraktijk-zaandam-180596</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>Tandartspraktijk Romero</t>
-        </is>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartspraktijk-romero-honselersdijk-10027597</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>De Tandarts, kliniek voor tandheelkunde en implantologie</t>
-        </is>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-de-tandarts-kliniek-voor-tandheelkunde-en-implantologie-raamsdonksveer-184568</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>Operatandarts de By &amp; de By</t>
-        </is>
-      </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-operatandarts-de-by-de-by-amsterdam-209685</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>Mondzorg Oosterhout</t>
-        </is>
-      </c>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-mondzorg-oosterhout-oosterhout-10026683</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>Tandartsenpraktijk Paul en de Witte</t>
-        </is>
-      </c>
-      <c r="C114" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartsenpraktijk-paul-en-de-witte-vlissingen-184137</t>
-        </is>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>Tandheelkunde Beverdam</t>
-        </is>
-      </c>
-      <c r="C115" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandheelkunde-beverdam-wierden-3036333</t>
-        </is>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>Dental Clinics Zaltbommel</t>
-        </is>
-      </c>
-      <c r="C116" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-zaltbommel-zaltbommel-208738</t>
-        </is>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>Tandartsenpraktijk Grou</t>
-        </is>
-      </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartsenpraktijk-grou-grou-188160</t>
-        </is>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>Dental Clinics Gouda Greenline</t>
-        </is>
-      </c>
-      <c r="C118" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-gouda-greenline-gouda-182093</t>
-        </is>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>PC2-tandartsen</t>
-        </is>
-      </c>
-      <c r="C119" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-pc2-tandartsen-eindhoven-3032943</t>
-        </is>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>Dental Clinics Beuningen</t>
-        </is>
-      </c>
-      <c r="C120" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-beuningen-beuningen-3046007</t>
-        </is>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="inlineStr">
-        <is>
-          <t>tandartsenpraktijk</t>
-        </is>
-      </c>
-      <c r="B121" t="inlineStr">
-        <is>
-          <t>Dental Clinics Colmschate</t>
-        </is>
-      </c>
-      <c r="C121" t="inlineStr">
-        <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-colmschate-colmschate-187204</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
enhance spider with dynamic start\_urls parsing, robust max\_page handling, and improved logging
</commit_message>
<xml_diff>
--- a/ZorgkaartScrapy/data/zorgkaart_organisaties.xlsx
+++ b/ZorgkaartScrapy/data/zorgkaart_organisaties.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -793,340 +793,340 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>tandartsenpraktijk</t>
+          <t>huisartsenpraktijk</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Tandarts A. Karic-Linic</t>
+          <t>Snipmeister</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandarts-a-karic-linic-den-haag-3042897</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-snipmeister-zeist-10021848</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>tandartsenpraktijk</t>
+          <t>huisartsenpraktijk</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Tandartsjordaan.nl</t>
+          <t>Huisartsen Assen-West</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartsjordaan-nl-amsterdam-3042877</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsen-assen-west-assen-10018454</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>tandartsenpraktijk</t>
+          <t>huisartsenpraktijk</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Omnident, Kliniek voor Tandheelkunde</t>
+          <t>Huisartspraktijk W. van Breugel</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-omnident-kliniek-voor-tandheelkunde-breda-237106</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartspraktijk-w-van-breugel-zevenhuizen-3035708</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>tandartsenpraktijk</t>
+          <t>huisartsenpraktijk</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>TandAnders</t>
+          <t>Huisartspraktijk Olieslagers</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandanders-raamsdonksveer-10001160</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartspraktijk-olieslagers-rockanje-118460</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>tandartsenpraktijk</t>
+          <t>huisartsenpraktijk</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Tandartspraktijk Biddinghuizen</t>
+          <t>Huisartsenpraktijk Arts en Zorg Leeuwarden</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartspraktijk-biddinghuizen-biddinghuizen-3056524</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-arts-en-zorg-leeuwarden-leeuwarden-3031757</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>tandartsenpraktijk</t>
+          <t>huisartsenpraktijk</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Tandartspraktijk Waldent</t>
+          <t>Huisartsenpraktijk Arts en Zorg Veldweg</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartspraktijk-waldent-den-haag-10002884</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-arts-en-zorg-veldweg-wezep-124911</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>tandartsenpraktijk</t>
+          <t>huisartsenpraktijk</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Tandarts De Ronde Venen</t>
+          <t>Huisartsenpraktijk Medi-Mere Buiten</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandarts-de-ronde-venen-mijdrecht-10025363</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-medi-mere-buiten-almere-3031382</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>tandartsenpraktijk</t>
+          <t>huisartsenpraktijk</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Allemans Tandartsen</t>
+          <t>Huisartsenpraktijk Arts en Zorg Gouden Hart</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-allemans-tandartsen-amerongen-10016011</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-arts-en-zorg-gouden-hart-berkel-en-rodenrijs-117268</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>tandartsenpraktijk</t>
+          <t>huisartsenpraktijk</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Tandheelkundig Centrum Kethel</t>
+          <t>Huisartsenpraktijk Arts en Zorg Jan Hendrik</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandheelkundig-centrum-kethel-schiedam-3055138</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-arts-en-zorg-jan-hendrik-den-haag-117092</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>tandartsenpraktijk</t>
+          <t>huisartsenpraktijk</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Tandartspraktijk Den Haag Centrum</t>
+          <t>Gezondheidscentrum Arts en Zorg Winschoten</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartspraktijk-den-haag-centrum-den-haag-3045011</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-gezondheidscentrum-arts-en-zorg-winschoten-winschoten-3034084</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>tandartsenpraktijk</t>
+          <t>huisartsenpraktijk</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Tandheelkundig Centrum Wilhelminapier</t>
+          <t>Huisartsenpraktijk Arts en Zorg Haagse Hout</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandheelkundig-centrum-wilhelminapier-rotterdam-181928</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-arts-en-zorg-haagse-hout-den-haag-3057129</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>tandartsenpraktijk</t>
+          <t>huisartsenpraktijk</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Tandartspraktijk De Weidevogel</t>
+          <t>Arts en Zorg</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartspraktijk-de-weidevogel-den-haag-3042694</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-arts-en-zorg-utrecht-10001581</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>tandartsenpraktijk</t>
+          <t>huisartsenpraktijk</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>SensaDent Tandartsen</t>
+          <t>Huisartsenpraktijken Medi-Mere</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-sensadent-tandartsen-amsterdam-3049885</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijken-medi-mere-almere-10026161</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>tandartsenpraktijk</t>
+          <t>huisartsenpraktijk</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>TPR | Tandartsenpraktijk Roelofarendsveen</t>
+          <t>Gezondheidscentrum Arts en Zorg Goudenregenhof</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tpr-tandartsenpraktijk-roelofarendsveen-roelofarendsveen-10017690</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-gezondheidscentrum-arts-en-zorg-goudenregenhof-den-haag-3006556</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>tandartsenpraktijk</t>
+          <t>huisartsenpraktijk</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Tandheelkundig Centrum Monnickendam, locatie De Haven</t>
+          <t>Gezondheidscentrum Arts en Zorg Hoendiep</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandheelkundig-centrum-monnickendam-locatie-de-haven-monnickendam-3042997</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-gezondheidscentrum-arts-en-zorg-hoendiep-groningen-251129</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>tandartsenpraktijk</t>
+          <t>huisartsenpraktijk</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Tandartspraktijk Kaptein en Hooykaas</t>
+          <t>Huisartsenpraktijk Arts en Zorg Vermeertoren</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartspraktijk-kaptein-en-hooykaas-hilversum-179678</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-arts-en-zorg-vermeertoren-delft-117171</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>tandartsenpraktijk</t>
+          <t>huisartsenpraktijk</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Tandartspraktijk Bas Hengeveld</t>
+          <t>Fonkelzorg Den Bosch</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartspraktijk-bas-hengeveld-weert-3033605</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-fonkelzorg-den-bosch-s-hertogenbosch-10022918</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>tandartsenpraktijk</t>
+          <t>huisartsenpraktijk</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Dental Clinics Beesd</t>
+          <t>Huisartspraktijk Waale</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-beesd-beesd-208613</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartspraktijk-waale-breda-205710</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>tandartsenpraktijk</t>
+          <t>huisartsenpraktijk</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>De Schans Tandartsen</t>
+          <t>Zorggroep Almere, Huisartsen</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-de-schans-tandartsen-leiden-10000705</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-zorggroep-almere-huisartsen-almere-10021227</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>tandartsenpraktijk</t>
+          <t>huisartsenpraktijk</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Tandartspraktijk Kirsten Knetsch</t>
+          <t>Huisartsenpraktijk A.A. van der Vaart</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartspraktijk-kirsten-knetsch-haarlem-178563</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-a-a-van-der-vaart-den-haag-3027638</t>
         </is>
       </c>
     </row>
@@ -1138,12 +1138,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Ferguson Hannewijk Tandartsen</t>
+          <t>Tandarts A. Karic-Linic</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-ferguson-hannewijk-tandartsen-rijnsburg-180935</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandarts-a-karic-linic-den-haag-3042897</t>
         </is>
       </c>
     </row>
@@ -1155,12 +1155,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Tandartsenpraktijk Zoeterwoudsesingel</t>
+          <t>Tandartsjordaan.nl</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartsenpraktijk-zoeterwoudsesingel-leiden-180956</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartsjordaan-nl-amsterdam-3042877</t>
         </is>
       </c>
     </row>
@@ -1172,12 +1172,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Tandheelkunde &amp; Implantologie Amsterdam</t>
+          <t>Omnident, Kliniek voor Tandheelkunde</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandheelkunde-implantologie-amsterdam-amsterdam-10026757</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-omnident-kliniek-voor-tandheelkunde-breda-237106</t>
         </is>
       </c>
     </row>
@@ -1189,12 +1189,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Tandheelkunde &amp; Implantologie Amsterdam, locatie Stadionweg</t>
+          <t>TandAnders</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandheelkunde-implantologie-amsterdam-locatie-stadionweg-amsterdam-178713</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandanders-raamsdonksveer-10001160</t>
         </is>
       </c>
     </row>
@@ -1206,12 +1206,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Tandartspraktijk Dronten</t>
+          <t>Tandartspraktijk Biddinghuizen</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartspraktijk-dronten-dronten-10017070</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartspraktijk-biddinghuizen-biddinghuizen-3056524</t>
         </is>
       </c>
     </row>
@@ -1223,12 +1223,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Tandartspraktijk Inge Schrauwen</t>
+          <t>Tandartspraktijk Waldent</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartspraktijk-inge-schrauwen-tilburg-3033485</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartspraktijk-waldent-den-haag-10002884</t>
         </is>
       </c>
     </row>
@@ -1240,12 +1240,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Dental Clinics Zandvoort</t>
+          <t>Tandarts De Ronde Venen</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-zandvoort-zandvoort-180752</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandarts-de-ronde-venen-mijdrecht-10025363</t>
         </is>
       </c>
     </row>
@@ -1257,12 +1257,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Mondzorgcentrum Takenhofplein</t>
+          <t>Allemans Tandartsen</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-mondzorgcentrum-takenhofplein-nijmegen-3059439</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-allemans-tandartsen-amerongen-10016011</t>
         </is>
       </c>
     </row>
@@ -1274,12 +1274,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Praktijk voor tandheelkunde en mondhygiëne Van Uijtert</t>
+          <t>Tandheelkundig Centrum Kethel</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-praktijk-voor-tandheelkunde-en-mondhygiene-van-uijtert-lage-zwaluwe-3035680</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandheelkundig-centrum-kethel-schiedam-3055138</t>
         </is>
       </c>
     </row>
@@ -1291,12 +1291,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Dental Clinics Purmerend de Gors</t>
+          <t>Tandartspraktijk Den Haag Centrum</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-purmerend-de-gors-purmerend-179617</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartspraktijk-den-haag-centrum-den-haag-3045011</t>
         </is>
       </c>
     </row>
@@ -1308,12 +1308,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>KTA Kliniek voor Tandheelkunde Amersfoort</t>
+          <t>Tandheelkundig Centrum Wilhelminapier</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-kta-kliniek-voor-tandheelkunde-amersfoort-amersfoort-3024325</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandheelkundig-centrum-wilhelminapier-rotterdam-181928</t>
         </is>
       </c>
     </row>
@@ -1325,12 +1325,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Tandartspraktijk De Jol Lelystad</t>
+          <t>Tandartspraktijk De Weidevogel</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartspraktijk-de-jol-lelystad-lelystad-3056450</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartspraktijk-de-weidevogel-den-haag-3042694</t>
         </is>
       </c>
     </row>
@@ -1342,12 +1342,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>DentXperts</t>
+          <t>SensaDent Tandartsen</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dentxperts-amsterdam-10005995</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-sensadent-tandartsen-amsterdam-3049885</t>
         </is>
       </c>
     </row>
@@ -1359,12 +1359,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Tandheelkundig Centrum Nederland Emmastraat</t>
+          <t>TPR | Tandartsenpraktijk Roelofarendsveen</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandheelkundig-centrum-nederland-emmastraat-alkmaar-180307</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tpr-tandartsenpraktijk-roelofarendsveen-roelofarendsveen-10017690</t>
         </is>
       </c>
     </row>
@@ -1376,12 +1376,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Mondzorg Aveling</t>
+          <t>Tandheelkundig Centrum Monnickendam, locatie De Haven</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-mondzorg-aveling-hoogvliet-10003794</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandheelkundig-centrum-monnickendam-locatie-de-haven-monnickendam-3042997</t>
         </is>
       </c>
     </row>
@@ -1393,12 +1393,12 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Tandartspraktijk Claessens</t>
+          <t>Tandartspraktijk Kaptein en Hooykaas</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartspraktijk-claessens-echt-185745</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartspraktijk-kaptein-en-hooykaas-hilversum-179678</t>
         </is>
       </c>
     </row>
@@ -1410,12 +1410,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Tandheelkundig Centrum Koraalzwam</t>
+          <t>Tandartspraktijk Bas Hengeveld</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandheelkundig-centrum-koraalzwam-alphen-aan-den-rijn-3041017</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartspraktijk-bas-hengeveld-weert-3033605</t>
         </is>
       </c>
     </row>
@@ -1427,12 +1427,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Mondzorg Maarssen</t>
+          <t>Dental Clinics Beesd</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-mondzorg-maarssen-maarssen-179758</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-beesd-beesd-208613</t>
         </is>
       </c>
     </row>
@@ -1444,12 +1444,12 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Tandartsenpraktijk Steyl</t>
+          <t>De Schans Tandartsen</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartsenpraktijk-steyl-steyl-185551</t>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-de-schans-tandartsen-leiden-10000705</t>
         </is>
       </c>
     </row>
@@ -1461,12 +1461,1032 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
+          <t>Tandartspraktijk Kirsten Knetsch</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartspraktijk-kirsten-knetsch-haarlem-178563</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Huisartsenpraktijk Haverkamp/Bastick</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-haverkamp-bastick-oosterhout-10005075</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Dokters van Hier</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-dokters-van-hier-maastricht-10013414</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Huisartsenpraktijk Kasbergen</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-kasbergen-lunteren-208193</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Huisartsenpraktijk van Elsen</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-van-elsen-oisterwijk-10019665</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Apotheekhoudende huisartsenpraktijk J.E. de Groot</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-apotheekhoudende-huisartsenpraktijk-j-e-de-groot-zuid-beijerland-3060002</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Huisartsenpraktijk Boddeus en Steenbergen</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-boddeus-en-steenbergen-groningen-126018</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Huisartspraktijk Van Eijk</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartspraktijk-van-eijk-delft-207863</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Huisartsen Kievit</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsen-kievit-bussum-205922</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Huisartsenpraktijk Binck-Zorg</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-binck-zorg-den-haag-10020425</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Huisartsenpraktijk Boas &amp; Valkenburg</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-boas-valkenburg-vianen-10012743</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Huisartsenpraktijk Kemper en Oldenburg</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-kemper-en-oldenburg-alkmaar-206554</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Huisartsenpraktijk Ridha</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-ridha-volendam-3048383</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Huisartsenpraktijk Trompert</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-trompert-zuidhorn-207393</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Huisartsenpraktijk Uitvindersbuurt</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-uitvindersbuurt-ede-123316</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>ClydesCure, Huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-clydescure-huisartsenpraktijk-lelystad-10082191</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Huisartsenpraktijk Blessing - Jeuring - Moonen</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-blessing-jeuring-moonen-udenhout-120894</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Huisartsenpraktijk Bongers</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-bongers-zeewolde-207820</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Huisartsenpraktijk De Diependaal</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-de-diependaal-stein-237109</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Huisartsenpraktijk De Dolfijn</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-de-dolfijn-middelburg-120118</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Huisartsenpraktijk De Hooge Boom</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-de-hooge-boom-hoogwoud-3005987</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Ferguson Hannewijk Tandartsen</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-ferguson-hannewijk-tandartsen-rijnsburg-180935</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Tandartsenpraktijk Zoeterwoudsesingel</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartsenpraktijk-zoeterwoudsesingel-leiden-180956</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Tandheelkunde &amp; Implantologie Amsterdam</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandheelkunde-implantologie-amsterdam-amsterdam-10026757</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Tandheelkunde &amp; Implantologie Amsterdam, locatie Stadionweg</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandheelkunde-implantologie-amsterdam-locatie-stadionweg-amsterdam-178713</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Tandartspraktijk Dronten</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartspraktijk-dronten-dronten-10017070</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Tandartspraktijk Inge Schrauwen</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartspraktijk-inge-schrauwen-tilburg-3033485</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Dental Clinics Zandvoort</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-zandvoort-zandvoort-180752</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Mondzorgcentrum Takenhofplein</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-mondzorgcentrum-takenhofplein-nijmegen-3059439</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Praktijk voor tandheelkunde en mondhygiëne Van Uijtert</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-praktijk-voor-tandheelkunde-en-mondhygiene-van-uijtert-lage-zwaluwe-3035680</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Dental Clinics Purmerend de Gors</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dental-clinics-purmerend-de-gors-purmerend-179617</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>KTA Kliniek voor Tandheelkunde Amersfoort</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-kta-kliniek-voor-tandheelkunde-amersfoort-amersfoort-3024325</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Tandartspraktijk De Jol Lelystad</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartspraktijk-de-jol-lelystad-lelystad-3056450</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>DentXperts</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-dentxperts-amsterdam-10005995</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Tandheelkundig Centrum Nederland Emmastraat</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandheelkundig-centrum-nederland-emmastraat-alkmaar-180307</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Mondzorg Aveling</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-mondzorg-aveling-hoogvliet-10003794</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Tandartspraktijk Claessens</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartspraktijk-claessens-echt-185745</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Tandheelkundig Centrum Koraalzwam</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandheelkundig-centrum-koraalzwam-alphen-aan-den-rijn-3041017</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Mondzorg Maarssen</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-mondzorg-maarssen-maarssen-179758</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Tandartsenpraktijk Steyl</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-tandartsenpraktijk-steyl-steyl-185551</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>tandartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
           <t>Top Dental</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr">
+      <c r="C101" t="inlineStr">
         <is>
           <t>https://www.zorgkaartnederland.nl/zorginstelling/tandartsenpraktijk-top-dental-volendam-3049583</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Huisartsenpraktijk Havekes</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-havekes-harderwijk-10019799</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Huisartsenpraktijk Het Zorgkwartier</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-het-zorgkwartier-ommen-124533</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Huisartsenpraktijk J.P. van Tussenbroek</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-j-p-van-tussenbroek-delft-117233</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Huisartsenpraktijk Majdandzic</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-majdandzic-breda-205739</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Huisartsenpraktijk Ritter en Kuipers</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-ritter-en-kuipers-rotterdam-208445</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Huisartsenpraktijk Schoterpoort, Praktijk Steketee</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-schoterpoort-praktijk-steketee-haarlem-3046049</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Huisartsenpraktijk Tabak</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-tabak-amsterdam-3046193</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Huisartsenpraktijk Ulestraten</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-ulestraten-ulestraten-3031904</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Huisartsenpraktijk van Beijsterveldt, locatie Dorst</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-van-beijsterveldt-locatie-dorst-dorst-120647</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Huisartsenpraktijk Vlaslant, Praktijk Verhoeckx</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-vlaslant-praktijk-verhoeckx-valkenswaard-10010787</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Huisartsenpraktijk Willems</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-willems-best-3056625</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Huisartsenpraktijk ZorghoekWestland</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartsenpraktijk-zorghoekwestland-honselersdijk-10001572</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Huisartspraktijk L. van Eijk</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartspraktijk-l-van-eijk-den-dolder-3037015</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Huisartspraktijk Willemsen</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-huisartspraktijk-willemsen-capelle-aan-den-ijssel-117569</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Apotheekhoudende Huisartsenpraktijk De Krim</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-apotheekhoudende-huisartsenpraktijk-de-krim-de-krim-124570</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Apotheekhoudende Huisartsenpraktijk Feij en Van der Wal</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-apotheekhoudende-huisartsenpraktijk-feij-en-van-der-wal-slochteren-3046266</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Apotheekhoudende huisartspraktijk J. de Kroon</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-apotheekhoudende-huisartspraktijk-j-de-kroon-onstwedde-207076</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>De Bergense Huisartsen- Praktijk Visser</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-de-bergense-huisartsen-praktijk-visser-bergen-3043935</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>De Colvenier, Huisartspraktijk D.H.A. Pons</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-de-colvenier-huisartspraktijk-d-h-a-pons-gorinchem-120010</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>huisartsenpraktijk</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>GCM Gezondheidscentrum Boomstede, Huisartsen</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>https://www.zorgkaartnederland.nl/zorginstelling/huisartsenpraktijk-gcm-gezondheidscentrum-boomstede-huisartsen-maarssen-102611</t>
         </is>
       </c>
     </row>

</xml_diff>